<commit_message>
add log to test data
</commit_message>
<xml_diff>
--- a/auto_USB_stress_test/Export_data xxxxxxx.xlsx
+++ b/auto_USB_stress_test/Export_data xxxxxxx.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="33">
   <si>
     <t>Duration</t>
   </si>
@@ -85,40 +85,34 @@
     <t>0</t>
   </si>
   <si>
-    <t>295.45</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>295.44</t>
+  </si>
+  <si>
+    <t>295.42</t>
+  </si>
+  <si>
+    <t>295.39</t>
+  </si>
+  <si>
+    <t>295.41</t>
+  </si>
+  <si>
+    <t>295.59</t>
   </si>
   <si>
     <t>295.37</t>
   </si>
   <si>
-    <t>295.52</t>
-  </si>
-  <si>
-    <t>295.49</t>
-  </si>
-  <si>
     <t>295.38</t>
   </si>
   <si>
     <t>295.43</t>
   </si>
   <si>
-    <t>295.34</t>
-  </si>
-  <si>
-    <t>295.39</t>
-  </si>
-  <si>
-    <t>295.42</t>
-  </si>
-  <si>
-    <t>295.41</t>
-  </si>
-  <si>
-    <t>295.61</t>
-  </si>
-  <si>
-    <t>295.40</t>
+    <t>295.60</t>
   </si>
 </sst>
 </file>
@@ -476,7 +470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -546,7 +540,7 @@
         <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
         <v>22</v>
@@ -587,7 +581,7 @@
         <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
@@ -628,7 +622,7 @@
         <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J4" t="s">
         <v>22</v>
@@ -666,10 +660,10 @@
         <v>22</v>
       </c>
       <c r="H5">
-        <v>30</v>
+        <v>29.99</v>
       </c>
       <c r="I5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
         <v>22</v>
@@ -707,10 +701,10 @@
         <v>22</v>
       </c>
       <c r="H6">
-        <v>30</v>
+        <v>29.99</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J6" t="s">
         <v>22</v>
@@ -748,10 +742,10 @@
         <v>22</v>
       </c>
       <c r="H7">
-        <v>30</v>
+        <v>29.99</v>
       </c>
       <c r="I7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J7" t="s">
         <v>22</v>
@@ -789,10 +783,10 @@
         <v>22</v>
       </c>
       <c r="H8">
-        <v>30</v>
+        <v>29.99</v>
       </c>
       <c r="I8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J8" t="s">
         <v>22</v>
@@ -830,7 +824,7 @@
         <v>22</v>
       </c>
       <c r="H9">
-        <v>30</v>
+        <v>29.99</v>
       </c>
       <c r="I9" t="s">
         <v>29</v>
@@ -871,10 +865,10 @@
         <v>22</v>
       </c>
       <c r="H10">
-        <v>30</v>
+        <v>29.99</v>
       </c>
       <c r="I10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J10" t="s">
         <v>22</v>
@@ -912,10 +906,10 @@
         <v>22</v>
       </c>
       <c r="H11">
-        <v>30</v>
+        <v>29.99</v>
       </c>
       <c r="I11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J11" t="s">
         <v>22</v>
@@ -941,7 +935,7 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -956,7 +950,7 @@
         <v>30</v>
       </c>
       <c r="I12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J12" t="s">
         <v>22</v>
@@ -982,7 +976,7 @@
         <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -997,7 +991,7 @@
         <v>30</v>
       </c>
       <c r="I13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J13" t="s">
         <v>22</v>
@@ -1023,7 +1017,7 @@
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1038,7 +1032,7 @@
         <v>30</v>
       </c>
       <c r="I14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J14" t="s">
         <v>22</v>
@@ -1064,7 +1058,7 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1079,7 +1073,7 @@
         <v>30</v>
       </c>
       <c r="I15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J15" t="s">
         <v>22</v>
@@ -1105,7 +1099,7 @@
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1120,7 +1114,7 @@
         <v>30</v>
       </c>
       <c r="I16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J16" t="s">
         <v>22</v>
@@ -1146,7 +1140,7 @@
         <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1161,7 +1155,7 @@
         <v>30</v>
       </c>
       <c r="I17" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="J17" t="s">
         <v>22</v>
@@ -1187,7 +1181,7 @@
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1202,7 +1196,7 @@
         <v>30</v>
       </c>
       <c r="I18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J18" t="s">
         <v>22</v>
@@ -1214,47 +1208,6 @@
         <v>22</v>
       </c>
       <c r="M18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>8</v>
-      </c>
-      <c r="C19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19">
-        <v>30</v>
-      </c>
-      <c r="I19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J19" t="s">
-        <v>22</v>
-      </c>
-      <c r="K19" t="s">
-        <v>22</v>
-      </c>
-      <c r="L19" t="s">
-        <v>22</v>
-      </c>
-      <c r="M19" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>